<commit_message>
new event planet hatch
</commit_message>
<xml_diff>
--- a/input/event.xlsx
+++ b/input/event.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950A410F-51BC-445F-B3B0-C6EC310212F8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" tabRatio="797" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="797" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <definedName name="loc_coor">'Loc Coordinates'!$B$3:$E$40</definedName>
     <definedName name="Project_Name">Notes!$B$1</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="78">
   <si>
     <t>Name of project</t>
   </si>
@@ -254,22 +253,28 @@
     <t>Second Meeting</t>
   </si>
   <si>
-    <t>Where we hang out and further explore the world of Data Science.</t>
-  </si>
-  <si>
     <t>Planet Hatch</t>
   </si>
   <si>
-    <t>140 - 50 Crowther Ln, Fredericton, NB E3C 0J1</t>
-  </si>
-  <si>
-    <t>no schedule yet</t>
+    <t>Kaggle Competition</t>
+  </si>
+  <si>
+    <t>Planning next meetup</t>
+  </si>
+  <si>
+    <t>This meetup will be for practitioners interested in building on their skillsets.  All capabilities welcome.  We will be picking a Kaggle competition to work on.</t>
+  </si>
+  <si>
+    <t>Learn, share, be challenged, grow, network and have fun.</t>
+  </si>
+  <si>
+    <t>140 - 50 Crowther Lane, Fredericton, NB E3C 0J1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
@@ -428,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -488,9 +493,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2309,20 +2311,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2330,10 +2332,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2341,10 +2343,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -2352,10 +2354,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2363,7 +2365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -2382,14 +2384,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2397,25 +2399,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.453125" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.54296875" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" customWidth="1"/>
-    <col min="16" max="16" width="6.81640625" customWidth="1"/>
-    <col min="17" max="17" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
@@ -2423,7 +2425,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>36</v>
       </c>
@@ -2437,7 +2439,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -2447,7 +2449,7 @@
       </c>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -2457,7 +2459,7 @@
       </c>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -2467,7 +2469,7 @@
       </c>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>48</v>
       </c>
@@ -2477,7 +2479,7 @@
       </c>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>49</v>
       </c>
@@ -2487,7 +2489,7 @@
       </c>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>50</v>
       </c>
@@ -2497,7 +2499,7 @@
       </c>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>51</v>
       </c>
@@ -2507,7 +2509,7 @@
       </c>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>52</v>
       </c>
@@ -2517,7 +2519,7 @@
       </c>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -2527,7 +2529,7 @@
       </c>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>41</v>
       </c>
@@ -2537,7 +2539,7 @@
       </c>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>42</v>
       </c>
@@ -2547,7 +2549,7 @@
       </c>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -2557,7 +2559,7 @@
       </c>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>11</v>
       </c>
@@ -2567,7 +2569,7 @@
       </c>
       <c r="R17" s="2"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>12</v>
       </c>
@@ -2579,7 +2581,7 @@
       </c>
       <c r="R18" s="2"/>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>13</v>
       </c>
@@ -2589,7 +2591,7 @@
       </c>
       <c r="R19" s="2"/>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>14</v>
       </c>
@@ -2599,7 +2601,7 @@
       </c>
       <c r="R20" s="2"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>60</v>
       </c>
@@ -2611,29 +2613,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6:O6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.54296875" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" style="25" customWidth="1"/>
+    <col min="1" max="1" width="1.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="25" customWidth="1"/>
     <col min="3" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="31.26953125" customWidth="1"/>
-    <col min="7" max="10" width="19.7265625" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" customWidth="1"/>
+    <col min="7" max="10" width="19.7109375" customWidth="1"/>
     <col min="11" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
-    <col min="14" max="15" width="11.26953125" customWidth="1"/>
-    <col min="16" max="16" width="9.453125" customWidth="1"/>
-    <col min="17" max="17" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.28515625" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M2" s="2">
         <v>2</v>
       </c>
@@ -2644,7 +2646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="26" t="s">
         <v>36</v>
       </c>
@@ -2697,7 +2699,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:18" s="20" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:18" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="27">
         <v>1</v>
       </c>
@@ -2749,7 +2751,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="2:18" s="20" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:18" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="27">
         <v>2</v>
       </c>
@@ -2806,7 +2808,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="2:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:18" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="27">
         <v>3</v>
       </c>
@@ -2838,11 +2840,11 @@
         <f t="shared" si="0"/>
         <v>600 Bishop Drive, Fredericton, NB E3C 0B4</v>
       </c>
-      <c r="N6" s="44">
+      <c r="N6" s="43">
         <f t="shared" si="0"/>
         <v>45.941000000000003</v>
       </c>
-      <c r="O6" s="44">
+      <c r="O6" s="43">
         <f t="shared" si="0"/>
         <v>-66.674000000000007</v>
       </c>
@@ -2856,7 +2858,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="2:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:18" ht="90" x14ac:dyDescent="0.25">
       <c r="B7" s="27">
         <v>4</v>
       </c>
@@ -2868,13 +2870,13 @@
       </c>
       <c r="E7" s="21"/>
       <c r="F7" s="21" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>57</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="21"/>
@@ -2882,19 +2884,19 @@
         <v>43399</v>
       </c>
       <c r="L7" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M7" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>140 - 50 Crowther Ln, Fredericton, NB E3C 0J1</v>
+        <v>140 - 50 Crowther Lane, Fredericton, NB E3C 0J1</v>
       </c>
       <c r="N7" s="24">
         <f t="shared" si="0"/>
-        <v>45.931562999999997</v>
+        <v>45.931604999999998</v>
       </c>
       <c r="O7" s="24">
         <f t="shared" si="0"/>
-        <v>-66.658212599999999</v>
+        <v>-66.658276000000001</v>
       </c>
       <c r="P7" s="21">
         <v>1</v>
@@ -2904,7 +2906,7 @@
       </c>
       <c r="R7" s="23"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="27"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21"/>
@@ -2923,7 +2925,7 @@
       <c r="Q8" s="21"/>
       <c r="R8" s="23"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="27"/>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
@@ -2942,7 +2944,7 @@
       <c r="Q9" s="21"/>
       <c r="R9" s="23"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="27"/>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
@@ -2961,7 +2963,7 @@
       <c r="Q10" s="21"/>
       <c r="R10" s="23"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="27"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -2980,7 +2982,7 @@
       <c r="Q11" s="21"/>
       <c r="R11" s="23"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="27"/>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
@@ -2999,7 +3001,7 @@
       <c r="Q12" s="21"/>
       <c r="R12" s="23"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="27"/>
       <c r="C13" s="21"/>
       <c r="D13" s="21"/>
@@ -3018,7 +3020,7 @@
       <c r="Q13" s="21"/>
       <c r="R13" s="23"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="27"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -3037,7 +3039,7 @@
       <c r="Q14" s="21"/>
       <c r="R14" s="23"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="27"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
@@ -3056,7 +3058,7 @@
       <c r="Q15" s="21"/>
       <c r="R15" s="23"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="27"/>
       <c r="C16" s="21"/>
       <c r="D16" s="21"/>
@@ -3075,7 +3077,7 @@
       <c r="Q16" s="21"/>
       <c r="R16" s="23"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="27"/>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
@@ -3094,7 +3096,7 @@
       <c r="Q17" s="21"/>
       <c r="R17" s="23"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="27"/>
       <c r="C18" s="21"/>
       <c r="D18" s="21"/>
@@ -3113,7 +3115,7 @@
       <c r="Q18" s="21"/>
       <c r="R18" s="23"/>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="27"/>
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
@@ -3132,7 +3134,7 @@
       <c r="Q19" s="21"/>
       <c r="R19" s="23"/>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="27"/>
       <c r="C20" s="21"/>
       <c r="D20" s="21"/>
@@ -3151,7 +3153,7 @@
       <c r="Q20" s="21"/>
       <c r="R20" s="23"/>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="27"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
@@ -3170,7 +3172,7 @@
       <c r="Q21" s="21"/>
       <c r="R21" s="23"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="27"/>
       <c r="C22" s="21"/>
       <c r="D22" s="21"/>
@@ -3189,7 +3191,7 @@
       <c r="Q22" s="21"/>
       <c r="R22" s="23"/>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="27"/>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
@@ -3208,7 +3210,7 @@
       <c r="Q23" s="21"/>
       <c r="R23" s="23"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="27"/>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
@@ -3227,7 +3229,7 @@
       <c r="Q24" s="21"/>
       <c r="R24" s="23"/>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="27"/>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
@@ -3246,7 +3248,7 @@
       <c r="Q25" s="21"/>
       <c r="R25" s="23"/>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="27"/>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
@@ -3265,7 +3267,7 @@
       <c r="Q26" s="21"/>
       <c r="R26" s="23"/>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="27"/>
       <c r="C27" s="21"/>
       <c r="D27" s="21"/>
@@ -3284,7 +3286,7 @@
       <c r="Q27" s="21"/>
       <c r="R27" s="23"/>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="27"/>
       <c r="C28" s="21"/>
       <c r="D28" s="21"/>
@@ -3303,7 +3305,7 @@
       <c r="Q28" s="21"/>
       <c r="R28" s="23"/>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="27"/>
       <c r="C29" s="21"/>
       <c r="D29" s="21"/>
@@ -3322,7 +3324,7 @@
       <c r="Q29" s="21"/>
       <c r="R29" s="23"/>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="27"/>
       <c r="C30" s="21"/>
       <c r="D30" s="21"/>
@@ -3341,7 +3343,7 @@
       <c r="Q30" s="21"/>
       <c r="R30" s="23"/>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="27"/>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
@@ -3360,8 +3362,8 @@
       <c r="Q31" s="21"/>
       <c r="R31" s="23"/>
     </row>
-    <row r="32" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="36"/>
+    <row r="32" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="35"/>
       <c r="C32" s="32"/>
       <c r="D32" s="30"/>
       <c r="E32" s="30"/>
@@ -3385,35 +3387,34 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.54296875" customWidth="1"/>
-    <col min="2" max="2" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>36</v>
       </c>
@@ -3466,7 +3467,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="34">
         <v>1</v>
       </c>
@@ -3513,7 +3514,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="34">
         <v>2</v>
       </c>
@@ -3569,387 +3570,405 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B6" s="43">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="42">
         <v>3</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C6" s="41">
         <v>0.70833333333333337</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="41">
         <v>0.72916666666666663</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="42">
+      <c r="F6" s="41">
         <v>0.72916666666666663</v>
       </c>
-      <c r="G6" s="42">
+      <c r="G6" s="41">
         <v>0.77083333333333337</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="40" t="s">
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="39" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B7" s="35"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="40" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B8" s="35"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="42">
+        <v>4</v>
+      </c>
+      <c r="C7" s="41">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D7" s="41">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="41">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="G7" s="41">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="41">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="J7" s="41">
+        <v>0.875</v>
+      </c>
+      <c r="K7" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="39"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="42"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
       <c r="R8" s="15"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B9" s="35"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="42"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
       <c r="R9" s="15"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B10" s="35"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="42"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
       <c r="R10" s="15"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B11" s="35"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="42"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
       <c r="R11" s="15"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B12" s="35"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="42"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
       <c r="R12" s="15"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B13" s="35"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="42"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
       <c r="R13" s="15"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B14" s="35"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="42"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
       <c r="R14" s="15"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B15" s="35"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="42"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
       <c r="R15" s="15"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B16" s="35"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="42"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
       <c r="R16" s="15"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B17" s="35"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B17" s="42"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
       <c r="R17" s="15"/>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B18" s="35"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B18" s="42"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
       <c r="R18" s="15"/>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B19" s="35"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B19" s="42"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
       <c r="R19" s="15"/>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B20" s="35"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B20" s="42"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
       <c r="R20" s="15"/>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B21" s="35"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B21" s="42"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="41"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
       <c r="R21" s="15"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B22" s="35"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B22" s="42"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
       <c r="R22" s="15"/>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B23" s="35"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B23" s="42"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="41"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
       <c r="R23" s="15"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B24" s="35"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B24" s="42"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
       <c r="R24" s="15"/>
     </row>
-    <row r="25" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="36"/>
+    <row r="25" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="35"/>
       <c r="C25" s="32"/>
       <c r="D25" s="31"/>
       <c r="E25" s="31"/>
@@ -3973,25 +3992,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.54296875" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>41</v>
       </c>
@@ -4005,7 +4024,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>38</v>
       </c>
@@ -4017,7 +4036,7 @@
         <v>-66.646332000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>43</v>
       </c>
@@ -4031,231 +4050,230 @@
         <v>-66.646791899999997</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="39" t="s">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="37">
         <v>45.941000000000003</v>
       </c>
       <c r="E6" s="12">
         <v>-66.674000000000007</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B7" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="38">
-        <v>45.931562999999997</v>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="37">
+        <v>45.931604999999998</v>
       </c>
       <c r="E7" s="12">
-        <f>G7+0.0005</f>
-        <v>-66.658212599999999</v>
-      </c>
-      <c r="G7" s="12">
+        <v>-66.658276000000001</v>
+      </c>
+      <c r="G7" s="37">
         <v>-66.658712600000001</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="14"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="15"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="14"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="15"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="14"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="15"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="15"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="14"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="15"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="15"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="15"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="14"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="15"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="15"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="14"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="15"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="14"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="15"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="14"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="15"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="14"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="15"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="14"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="15"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="14"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="15"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="14"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="15"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="14"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="15"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="14"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="15"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="14"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="15"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="14"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="15"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="14"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="15"/>
     </row>
-    <row r="40" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="16"/>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>

</xml_diff>